<commit_message>
edit exercises, add solutions Rmarkdown, add solutions to .gitignore
</commit_message>
<xml_diff>
--- a/data/sttstj_all_sites.xlsx
+++ b/data/sttstj_all_sites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20413"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremiah.blondeau\Documents\R\mmes\week_3_exercises\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1B1CFA-5573-4F0C-AF48-AB668690C6FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B87E1DC-329E-4A25-92B1-1FF6293129B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7577,9 +7577,6 @@
     <t>2001-2021 all fish sample locations</t>
   </si>
   <si>
-    <t>year and site id concatenated</t>
-  </si>
-  <si>
     <t>latitude</t>
   </si>
   <si>
@@ -7593,6 +7590,9 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>unique sample, year and site id concatenated</t>
   </si>
 </sst>
 </file>
@@ -7985,13 +7985,13 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -8011,10 +8011,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>2521</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>2522</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2523</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -8022,7 +8022,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2518</v>
+        <v>2523</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -8032,7 +8032,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -8042,7 +8042,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -8052,7 +8052,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>

</xml_diff>